<commit_message>
Round GDPGR values to an even multiple of the recession lever step size
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD721E-B280-4ED4-B6B9-3F92CB328231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="19418" windowHeight="10418"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
     <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -252,10 +253,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -356,7 +358,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -374,6 +375,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -655,29 +657,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.53125" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -685,237 +685,237 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -923,36 +923,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.53125" customWidth="1"/>
-    <col min="2" max="2" width="27.46484375" customWidth="1"/>
-    <col min="3" max="3" width="17.265625" customWidth="1"/>
-    <col min="4" max="7" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="7" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2019</v>
       </c>
@@ -962,14 +960,14 @@
       <c r="D2">
         <v>2021</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -982,14 +980,14 @@
       <c r="D3">
         <v>19194</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1002,57 +1000,57 @@
       <c r="D4">
         <v>19790</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="15" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <f>B3</f>
         <v>19073</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <f>C4*($B$3/$B$4)</f>
         <v>19453.099643381582</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <f>D4*($B$3/$B$4)</f>
         <v>19795.189322425005</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1064,59 +1062,59 @@
         <f>(D3-D5)/D5</f>
         <v>-3.0370476009741777E-2</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="15" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <f>C5/B5-1</f>
         <v>1.9928676316341543E-2</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <f>C3/B3-1</f>
         <v>-5.3950610811094202E-2</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,22 +1123,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.53125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -1148,11 +1144,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="22">
         <f>Data!B12</f>
         <v>-5.3950610811094202E-2</v>
       </c>
@@ -1163,22 +1159,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.53125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -1186,11 +1180,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="22">
         <f>Data!B11</f>
         <v>1.9928676316341543E-2</v>
       </c>

</xml_diff>

<commit_message>
Remove left-over draft text from About tab of ctrl-settings/GDPGR
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD721E-B280-4ED4-B6B9-3F92CB328231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E3D8B-4918-4FCD-B753-578DC20F9A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>About</t>
   </si>
@@ -59,29 +59,6 @@
     <t>broader set of input data.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This control lever adjusts the inputs in the model </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>relative to the data</t>
-    </r>
-  </si>
-  <si>
-    <t>here.  Instead, you specify an adjustment to energy demand and</t>
-  </si>
-  <si>
-    <t>economic activity relative to the levels of energy demand and activity</t>
-  </si>
-  <si>
     <t>for in the various input data files that govern energy demand, etc.</t>
   </si>
   <si>
@@ -97,46 +74,10 @@
     <t>under a economic growth forecast different from that assumed by the</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>entered in the other input variables</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.  It does not specify new economic</t>
-    </r>
-  </si>
-  <si>
-    <t>conditions on its own - that is, you don't specify a GDP growth rate</t>
-  </si>
-  <si>
-    <t>specified in the input dataset.</t>
-  </si>
-  <si>
     <t>Sources:</t>
   </si>
   <si>
     <t>U.S. GDP Impact of SARC-CoV-2 Pandemic</t>
-  </si>
-  <si>
-    <t>As of EPS 2.1.1, AEBC is set up to model the impacts of the 2020</t>
-  </si>
-  <si>
-    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of Apr 8,</t>
   </si>
   <si>
     <t>2020, but due to the rapidly evolving nature of the situation,</t>
@@ -257,9 +198,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,15 +217,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -340,21 +272,21 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -375,7 +307,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -658,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -669,45 +601,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +649,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,7 +659,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +669,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -757,17 +689,17 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,140 +709,84 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +814,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -969,7 +845,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>19073</v>
@@ -989,7 +865,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>19068</v>
@@ -1009,7 +885,7 @@
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <f>B3</f>
@@ -1032,7 +908,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -1052,7 +928,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5">
         <f>(C3-C5)/C5</f>
@@ -1079,7 +955,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1093,7 +969,7 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B11" s="12">
         <f>C5/B5-1</f>
@@ -1108,7 +984,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B12" s="12">
         <f>C3/B3-1</f>
@@ -1138,15 +1014,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B2" s="22">
         <f>Data!B12</f>
@@ -1174,15 +1050,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B2" s="22">
         <f>Data!B11</f>

</xml_diff>

<commit_message>
Update COVID recession files for July STEO
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E3D8B-4918-4FCD-B753-578DC20F9A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
     <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -152,9 +151,6 @@
     <t>Source: Tables 9a, row 1</t>
   </si>
   <si>
-    <t>May STEO</t>
-  </si>
-  <si>
     <t>Counterfactual GDP Growth Rate</t>
   </si>
   <si>
@@ -189,12 +185,15 @@
   </si>
   <si>
     <t>Real GDP (billion chained 2012 dollars)</t>
+  </si>
+  <si>
+    <t>July STEO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
@@ -589,27 +588,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -617,181 +616,181 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -799,22 +798,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="7" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="2" max="2" width="27.3984375" customWidth="1"/>
+    <col min="3" max="3" width="17.265625" customWidth="1"/>
+    <col min="4" max="7" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -826,7 +827,7 @@
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>2019</v>
       </c>
@@ -843,18 +844,18 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>19073</v>
       </c>
       <c r="C3">
-        <v>18044</v>
+        <v>17517</v>
       </c>
       <c r="D3">
-        <v>19194</v>
+        <v>18418</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -863,7 +864,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -883,9 +884,9 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <f>B3</f>
@@ -906,7 +907,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
@@ -917,7 +918,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D7" s="12"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -926,17 +927,17 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="5">
         <f>(C3-C5)/C5</f>
-        <v>-7.2435738736422492E-2</v>
+        <v>-9.952653710074888E-2</v>
       </c>
       <c r="D8" s="5">
         <f>(D3-D5)/D5</f>
-        <v>-3.0370476009741777E-2</v>
+        <v>-6.9571919722174844E-2</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
@@ -945,7 +946,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -953,9 +954,9 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -967,9 +968,9 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="12">
         <f>C5/B5-1</f>
@@ -982,13 +983,13 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="12">
         <f>C3/B3-1</f>
-        <v>-5.3950610811094202E-2</v>
+        <v>-8.1581292927174531E-2</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -999,7 +1000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1007,12 +1008,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -1020,13 +1021,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="22">
         <f>Data!B12</f>
-        <v>-5.3950610811094202E-2</v>
+        <v>-8.1581292927174531E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1043,12 +1044,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>